<commit_message>
Indicator otu tables with plant otus removed.
</commit_message>
<xml_diff>
--- a/Tables/Indicator_OTUs_table.xlsx
+++ b/Tables/Indicator_OTUs_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/liberjul_msu_edu/Documents/Documents/MSU/Undergrad/Fall 2018/PLP 847/miseq_dat/Leaf_litter_communities/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="8_{4525134C-F3F8-4522-AA44-BC08756F593C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{599DFCD4-1788-4D7B-B548-03CF587CE500}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{4525134C-F3F8-4522-AA44-BC08756F593C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9A4C4F56-0987-4D43-AC2F-2B1551CECF32}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{39DCFC5A-FC43-46D7-8741-D84C4CB1D525}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="120">
   <si>
     <t>Substrate</t>
   </si>
@@ -587,9 +587,6 @@
     </r>
   </si>
   <si>
-    <t>OTU_735</t>
-  </si>
-  <si>
     <t>Hypoxylon carneum</t>
   </si>
   <si>
@@ -966,25 +963,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Fungi</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> sp.</t>
-    </r>
+    <t>OTU_1104</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1386,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I8" sqref="I8"/>
+      <selection pane="topRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1447,8 +1426,8 @@
       <c r="C2" s="5">
         <v>3.3E-3</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>120</v>
+      <c r="D2" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>6</v>
@@ -1587,13 +1566,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="C11" s="3">
         <v>3.4466945606694603E-2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>9</v>
@@ -1613,7 +1592,7 @@
         <v>94</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1664,7 +1643,7 @@
         <v>85</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1679,7 +1658,7 @@
         <v>95</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1696,7 +1675,7 @@
         <v>75</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1713,7 +1692,7 @@
         <v>96</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1747,7 +1726,7 @@
         <v>73</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1762,7 +1741,7 @@
         <v>72</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.35">
@@ -1813,7 +1792,7 @@
         <v>85</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1879,7 +1858,7 @@
         <v>100</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1913,7 +1892,7 @@
         <v>80</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1945,7 +1924,7 @@
         <v>85</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1962,7 +1941,7 @@
         <v>88</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -2013,7 +1992,7 @@
         <v>81</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -2030,7 +2009,7 @@
         <v>82</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -2081,7 +2060,7 @@
         <v>83</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -2098,7 +2077,7 @@
         <v>49</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -2130,7 +2109,7 @@
         <v>90</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2143,6 +2122,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AFDA51084187F242B05EFA296C5963FF" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3643f2840fd34a552c287b84deed346">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3ea71f81-dc8a-4f4b-b0dd-c828e930e924" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc954b55e77a02dd874654cc5b225bc" ns3:_="">
     <xsd:import namespace="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
@@ -2326,35 +2320,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC6078DA-B410-4273-80BB-BA4B90A0F31E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CE91A7C-6955-4F6F-A8F8-9CC25BBFD0AA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2376,9 +2345,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CE91A7C-6955-4F6F-A8F8-9CC25BBFD0AA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC6078DA-B410-4273-80BB-BA4B90A0F31E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>